<commit_message>
Added manual required Hour Input.
</commit_message>
<xml_diff>
--- a/creator/forms_xlsx/DATASHEET.xlsx
+++ b/creator/forms_xlsx/DATASHEET.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\bprc_project\VM\tbpc_dev\tbpc\resource_mgt\forms_xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\odoo_dev\extra_addons\budget_outsource\creator\forms_xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9435"/>
   </bookViews>
   <sheets>
     <sheet name="STAFF LIST" sheetId="3" r:id="rId1"/>
@@ -1004,8 +1004,8 @@
   </sheetPr>
   <dimension ref="A1:Z12"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1279,7 +1279,7 @@
         <v>14</v>
       </c>
       <c r="R7" s="50">
-        <f>IF(ISBLANK(S7),0,ROUND((Q7-S7)*(48/7),0))</f>
+        <f>IF(ISBLANK(S7),0,ROUND((Q7-S7)*(P7/Q7),0))</f>
         <v>0</v>
       </c>
       <c r="S7" s="23"/>
@@ -1364,7 +1364,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="10" ySplit="6" topLeftCell="K7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>

</xml_diff>

<commit_message>
Fix:     - fix get_required_hour     - fix datasheet form to only show whole number for required hours
</commit_message>
<xml_diff>
--- a/creator/forms_xlsx/DATASHEET.xlsx
+++ b/creator/forms_xlsx/DATASHEET.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\odoo_dev\extra_addons\budget_outsource\creator\forms_xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\odoo_dev\_extra_addons\budget_outsource\creator\forms_xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -500,7 +500,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -684,6 +684,20 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1004,8 +1018,8 @@
   </sheetPr>
   <dimension ref="A1:Z12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="R7" sqref="R7"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="W8" sqref="W8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1024,7 +1038,7 @@
     <col min="13" max="13" width="13.42578125" style="1" customWidth="1"/>
     <col min="14" max="14" width="17.5703125" style="1" customWidth="1"/>
     <col min="15" max="15" width="15" style="1" customWidth="1"/>
-    <col min="16" max="16" width="17.85546875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="17.85546875" style="70" customWidth="1"/>
     <col min="17" max="17" width="17.85546875" style="1" hidden="1" customWidth="1"/>
     <col min="18" max="18" width="15.28515625" style="1" customWidth="1"/>
     <col min="19" max="19" width="8.5703125" style="1" customWidth="1"/>
@@ -1037,53 +1051,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="70" t="s">
+      <c r="B1" s="76" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
-      <c r="J1" s="70"/>
-      <c r="K1" s="70"/>
-      <c r="L1" s="70"/>
-      <c r="M1" s="70"/>
-      <c r="N1" s="70"/>
-      <c r="O1" s="70"/>
-      <c r="P1" s="70"/>
-      <c r="Q1" s="70"/>
-      <c r="R1" s="70"/>
-      <c r="S1" s="70"/>
-      <c r="T1" s="70"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
+      <c r="L1" s="76"/>
+      <c r="M1" s="76"/>
+      <c r="N1" s="76"/>
+      <c r="O1" s="76"/>
+      <c r="P1" s="76"/>
+      <c r="Q1" s="76"/>
+      <c r="R1" s="76"/>
+      <c r="S1" s="76"/>
+      <c r="T1" s="76"/>
       <c r="Z1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="71" t="s">
+      <c r="B2" s="77" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
-      <c r="L2" s="71"/>
-      <c r="M2" s="71"/>
-      <c r="N2" s="71"/>
-      <c r="O2" s="71"/>
-      <c r="P2" s="71"/>
-      <c r="Q2" s="71"/>
-      <c r="R2" s="71"/>
-      <c r="S2" s="71"/>
-      <c r="T2" s="71"/>
+      <c r="C2" s="77"/>
+      <c r="D2" s="77"/>
+      <c r="E2" s="77"/>
+      <c r="F2" s="77"/>
+      <c r="G2" s="77"/>
+      <c r="H2" s="77"/>
+      <c r="I2" s="77"/>
+      <c r="J2" s="77"/>
+      <c r="K2" s="77"/>
+      <c r="L2" s="77"/>
+      <c r="M2" s="77"/>
+      <c r="N2" s="77"/>
+      <c r="O2" s="77"/>
+      <c r="P2" s="77"/>
+      <c r="Q2" s="77"/>
+      <c r="R2" s="77"/>
+      <c r="S2" s="77"/>
+      <c r="T2" s="77"/>
       <c r="Z2" s="1" t="s">
         <v>15</v>
       </c>
@@ -1103,7 +1117,7 @@
       <c r="M3" s="51"/>
       <c r="N3" s="51"/>
       <c r="O3" s="51"/>
-      <c r="P3" s="51"/>
+      <c r="P3" s="65"/>
       <c r="Q3" s="51"/>
       <c r="R3" s="51"/>
       <c r="S3" s="51"/>
@@ -1124,7 +1138,7 @@
       <c r="M4" s="60"/>
       <c r="N4" s="60"/>
       <c r="O4" s="60"/>
-      <c r="P4" s="60"/>
+      <c r="P4" s="66"/>
       <c r="Q4" s="60"/>
       <c r="R4" s="63"/>
       <c r="S4" s="60"/>
@@ -1134,29 +1148,29 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="67" t="s">
+      <c r="B5" s="73" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="68"/>
-      <c r="D5" s="68"/>
-      <c r="E5" s="68"/>
-      <c r="F5" s="68"/>
-      <c r="G5" s="68"/>
-      <c r="H5" s="68"/>
-      <c r="I5" s="68"/>
-      <c r="J5" s="68"/>
-      <c r="K5" s="68"/>
-      <c r="L5" s="68"/>
-      <c r="M5" s="68"/>
-      <c r="N5" s="68"/>
-      <c r="O5" s="68"/>
-      <c r="P5" s="69"/>
+      <c r="C5" s="74"/>
+      <c r="D5" s="74"/>
+      <c r="E5" s="74"/>
+      <c r="F5" s="74"/>
+      <c r="G5" s="74"/>
+      <c r="H5" s="74"/>
+      <c r="I5" s="74"/>
+      <c r="J5" s="74"/>
+      <c r="K5" s="74"/>
+      <c r="L5" s="74"/>
+      <c r="M5" s="74"/>
+      <c r="N5" s="74"/>
+      <c r="O5" s="74"/>
+      <c r="P5" s="75"/>
       <c r="Q5" s="58"/>
-      <c r="R5" s="65" t="s">
+      <c r="R5" s="71" t="s">
         <v>10</v>
       </c>
-      <c r="S5" s="65"/>
-      <c r="T5" s="66"/>
+      <c r="S5" s="71"/>
+      <c r="T5" s="72"/>
       <c r="Z5" s="1" t="s">
         <v>15</v>
       </c>
@@ -1204,7 +1218,7 @@
       <c r="O6" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="P6" s="54" t="s">
+      <c r="P6" s="67" t="s">
         <v>3</v>
       </c>
       <c r="Q6" s="54" t="s">
@@ -1272,7 +1286,7 @@
       <c r="O7" s="19">
         <v>13</v>
       </c>
-      <c r="P7" s="19">
+      <c r="P7" s="68">
         <v>14</v>
       </c>
       <c r="Q7" s="19">
@@ -1285,7 +1299,7 @@
       <c r="S7" s="23"/>
       <c r="T7" s="49"/>
       <c r="W7" s="15">
-        <f>R7/P7</f>
+        <f>R7/ROUND(P7,0)</f>
         <v>0</v>
       </c>
       <c r="X7" s="15">
@@ -1312,7 +1326,7 @@
       <c r="M8" s="14"/>
       <c r="N8" s="14"/>
       <c r="O8" s="14"/>
-      <c r="P8" s="20"/>
+      <c r="P8" s="69"/>
       <c r="Q8" s="20"/>
       <c r="R8" s="20"/>
       <c r="S8" s="21" t="str">
@@ -1398,51 +1412,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="70" t="str">
+      <c r="B1" s="76" t="str">
         <f>'STAFF LIST'!B1:T1</f>
         <v>713H CLAIMS FOR VENDOR NAME</v>
       </c>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
-      <c r="J1" s="70"/>
-      <c r="K1" s="70"/>
-      <c r="L1" s="70"/>
-      <c r="M1" s="70"/>
-      <c r="N1" s="70"/>
-      <c r="O1" s="70"/>
-      <c r="P1" s="70"/>
-      <c r="Q1" s="70"/>
-      <c r="R1" s="70"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
+      <c r="L1" s="76"/>
+      <c r="M1" s="76"/>
+      <c r="N1" s="76"/>
+      <c r="O1" s="76"/>
+      <c r="P1" s="76"/>
+      <c r="Q1" s="76"/>
+      <c r="R1" s="76"/>
       <c r="X1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:24" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="71" t="str">
+      <c r="B2" s="77" t="str">
         <f>'STAFF LIST'!B2:T2</f>
         <v>Aug-16 to Sep-16</v>
       </c>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
-      <c r="L2" s="71"/>
-      <c r="M2" s="71"/>
-      <c r="N2" s="71"/>
-      <c r="O2" s="71"/>
-      <c r="P2" s="71"/>
-      <c r="Q2" s="71"/>
-      <c r="R2" s="71"/>
+      <c r="C2" s="77"/>
+      <c r="D2" s="77"/>
+      <c r="E2" s="77"/>
+      <c r="F2" s="77"/>
+      <c r="G2" s="77"/>
+      <c r="H2" s="77"/>
+      <c r="I2" s="77"/>
+      <c r="J2" s="77"/>
+      <c r="K2" s="77"/>
+      <c r="L2" s="77"/>
+      <c r="M2" s="77"/>
+      <c r="N2" s="77"/>
+      <c r="O2" s="77"/>
+      <c r="P2" s="77"/>
+      <c r="Q2" s="77"/>
+      <c r="R2" s="77"/>
       <c r="X2" s="1" t="s">
         <v>15</v>
       </c>
@@ -1489,27 +1503,27 @@
       </c>
     </row>
     <row r="5" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="72" t="s">
+      <c r="B5" s="78" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="73"/>
-      <c r="D5" s="73"/>
-      <c r="E5" s="73"/>
-      <c r="F5" s="73"/>
-      <c r="G5" s="73"/>
-      <c r="H5" s="73"/>
-      <c r="I5" s="73"/>
-      <c r="J5" s="73"/>
-      <c r="K5" s="73"/>
-      <c r="L5" s="73"/>
-      <c r="M5" s="73"/>
-      <c r="N5" s="73"/>
-      <c r="O5" s="73"/>
-      <c r="P5" s="74" t="s">
+      <c r="C5" s="79"/>
+      <c r="D5" s="79"/>
+      <c r="E5" s="79"/>
+      <c r="F5" s="79"/>
+      <c r="G5" s="79"/>
+      <c r="H5" s="79"/>
+      <c r="I5" s="79"/>
+      <c r="J5" s="79"/>
+      <c r="K5" s="79"/>
+      <c r="L5" s="79"/>
+      <c r="M5" s="79"/>
+      <c r="N5" s="79"/>
+      <c r="O5" s="79"/>
+      <c r="P5" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="Q5" s="74"/>
-      <c r="R5" s="75"/>
+      <c r="Q5" s="80"/>
+      <c r="R5" s="81"/>
       <c r="X5" s="1" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
Added Manager and Director
</commit_message>
<xml_diff>
--- a/creator/forms_xlsx/DATASHEET.xlsx
+++ b/creator/forms_xlsx/DATASHEET.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\odoo_dev\_extra_addons\budget_outsource\creator\forms_xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\odoo_dev\_addons_etisalat_11\budget_outsource\creator\forms_xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">MISMATCH!$B$6:$R$6</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'STAFF LIST'!$B$6:$T$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'STAFF LIST'!$B$6:$U$6</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="27">
   <si>
     <t>ResID</t>
   </si>
@@ -121,6 +121,9 @@
   </si>
   <si>
     <t>PO Number</t>
+  </si>
+  <si>
+    <t>Director</t>
   </si>
 </sst>
 </file>
@@ -500,7 +503,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -698,6 +701,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1016,10 +1022,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Z12"/>
+  <dimension ref="A1:AA12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="W8" sqref="W8"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="V7" sqref="V7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1028,86 +1034,88 @@
     <col min="2" max="2" width="7.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="1" customWidth="1"/>
     <col min="4" max="4" width="15.140625" style="24" customWidth="1"/>
-    <col min="5" max="5" width="39.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="7.5703125" style="1" customWidth="1"/>
-    <col min="7" max="8" width="12" style="1" customWidth="1"/>
-    <col min="9" max="9" width="12.5703125" style="28" customWidth="1"/>
-    <col min="10" max="10" width="17.28515625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="44.140625" style="24" customWidth="1"/>
-    <col min="12" max="12" width="21.42578125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="13.42578125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="17.5703125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="15" style="1" customWidth="1"/>
-    <col min="16" max="16" width="17.85546875" style="70" customWidth="1"/>
-    <col min="17" max="17" width="17.85546875" style="1" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="15.28515625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="8.5703125" style="1" customWidth="1"/>
-    <col min="20" max="20" width="40" style="1" customWidth="1"/>
-    <col min="21" max="22" width="9.140625" style="1"/>
-    <col min="23" max="23" width="11" style="1" customWidth="1"/>
-    <col min="24" max="25" width="9.140625" style="1" customWidth="1"/>
-    <col min="26" max="26" width="9.140625" style="1" hidden="1" customWidth="1"/>
-    <col min="27" max="16384" width="9.140625" style="1"/>
+    <col min="5" max="6" width="39.5703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5703125" style="1" customWidth="1"/>
+    <col min="8" max="9" width="12" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" style="28" customWidth="1"/>
+    <col min="11" max="11" width="17.28515625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="44.140625" style="24" customWidth="1"/>
+    <col min="13" max="13" width="21.42578125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="13.42578125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="17.5703125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="15" style="1" customWidth="1"/>
+    <col min="17" max="17" width="17.85546875" style="70" customWidth="1"/>
+    <col min="18" max="18" width="17.85546875" style="1" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="15.28515625" style="1" customWidth="1"/>
+    <col min="20" max="20" width="8.5703125" style="1" customWidth="1"/>
+    <col min="21" max="21" width="40" style="1" customWidth="1"/>
+    <col min="22" max="23" width="9.140625" style="1"/>
+    <col min="24" max="24" width="11" style="1" customWidth="1"/>
+    <col min="25" max="26" width="9.140625" style="1" customWidth="1"/>
+    <col min="27" max="27" width="9.140625" style="1" hidden="1" customWidth="1"/>
+    <col min="28" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="76" t="s">
+    <row r="1" spans="1:27" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="77" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="76"/>
-      <c r="H1" s="76"/>
-      <c r="I1" s="76"/>
-      <c r="J1" s="76"/>
-      <c r="K1" s="76"/>
-      <c r="L1" s="76"/>
-      <c r="M1" s="76"/>
-      <c r="N1" s="76"/>
-      <c r="O1" s="76"/>
-      <c r="P1" s="76"/>
-      <c r="Q1" s="76"/>
-      <c r="R1" s="76"/>
-      <c r="S1" s="76"/>
-      <c r="T1" s="76"/>
-      <c r="Z1" s="1" t="s">
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="77"/>
+      <c r="L1" s="77"/>
+      <c r="M1" s="77"/>
+      <c r="N1" s="77"/>
+      <c r="O1" s="77"/>
+      <c r="P1" s="77"/>
+      <c r="Q1" s="77"/>
+      <c r="R1" s="77"/>
+      <c r="S1" s="77"/>
+      <c r="T1" s="77"/>
+      <c r="U1" s="77"/>
+      <c r="AA1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="77" t="s">
+    <row r="2" spans="1:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="77"/>
-      <c r="D2" s="77"/>
-      <c r="E2" s="77"/>
-      <c r="F2" s="77"/>
-      <c r="G2" s="77"/>
-      <c r="H2" s="77"/>
-      <c r="I2" s="77"/>
-      <c r="J2" s="77"/>
-      <c r="K2" s="77"/>
-      <c r="L2" s="77"/>
-      <c r="M2" s="77"/>
-      <c r="N2" s="77"/>
-      <c r="O2" s="77"/>
-      <c r="P2" s="77"/>
-      <c r="Q2" s="77"/>
-      <c r="R2" s="77"/>
-      <c r="S2" s="77"/>
-      <c r="T2" s="77"/>
-      <c r="Z2" s="1" t="s">
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="78"/>
+      <c r="K2" s="78"/>
+      <c r="L2" s="78"/>
+      <c r="M2" s="78"/>
+      <c r="N2" s="78"/>
+      <c r="O2" s="78"/>
+      <c r="P2" s="78"/>
+      <c r="Q2" s="78"/>
+      <c r="R2" s="78"/>
+      <c r="S2" s="78"/>
+      <c r="T2" s="78"/>
+      <c r="U2" s="78"/>
+      <c r="AA2" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="51"/>
       <c r="C3" s="51"/>
       <c r="D3" s="51"/>
       <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
+      <c r="F3" s="71"/>
       <c r="G3" s="51"/>
       <c r="H3" s="51"/>
       <c r="I3" s="51"/>
@@ -1117,13 +1125,14 @@
       <c r="M3" s="51"/>
       <c r="N3" s="51"/>
       <c r="O3" s="51"/>
-      <c r="P3" s="65"/>
-      <c r="Q3" s="51"/>
+      <c r="P3" s="51"/>
+      <c r="Q3" s="65"/>
       <c r="R3" s="51"/>
       <c r="S3" s="51"/>
       <c r="T3" s="51"/>
-    </row>
-    <row r="4" spans="1:26" ht="33" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U3" s="51"/>
+    </row>
+    <row r="4" spans="1:27" ht="33" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="59"/>
       <c r="C4" s="60"/>
       <c r="D4" s="61"/>
@@ -1131,51 +1140,53 @@
       <c r="F4" s="60"/>
       <c r="G4" s="60"/>
       <c r="H4" s="60"/>
-      <c r="I4" s="62"/>
-      <c r="J4" s="60"/>
-      <c r="K4" s="61"/>
-      <c r="L4" s="60"/>
+      <c r="I4" s="60"/>
+      <c r="J4" s="62"/>
+      <c r="K4" s="60"/>
+      <c r="L4" s="61"/>
       <c r="M4" s="60"/>
       <c r="N4" s="60"/>
       <c r="O4" s="60"/>
-      <c r="P4" s="66"/>
-      <c r="Q4" s="60"/>
-      <c r="R4" s="63"/>
-      <c r="S4" s="60"/>
-      <c r="T4" s="64"/>
-      <c r="Z4" s="1" t="s">
+      <c r="P4" s="60"/>
+      <c r="Q4" s="66"/>
+      <c r="R4" s="60"/>
+      <c r="S4" s="63"/>
+      <c r="T4" s="60"/>
+      <c r="U4" s="64"/>
+      <c r="AA4" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="73" t="s">
+    <row r="5" spans="1:27" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="74" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="74"/>
-      <c r="D5" s="74"/>
-      <c r="E5" s="74"/>
-      <c r="F5" s="74"/>
-      <c r="G5" s="74"/>
-      <c r="H5" s="74"/>
-      <c r="I5" s="74"/>
-      <c r="J5" s="74"/>
-      <c r="K5" s="74"/>
-      <c r="L5" s="74"/>
-      <c r="M5" s="74"/>
-      <c r="N5" s="74"/>
-      <c r="O5" s="74"/>
+      <c r="C5" s="75"/>
+      <c r="D5" s="75"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="75"/>
+      <c r="G5" s="75"/>
+      <c r="H5" s="75"/>
+      <c r="I5" s="75"/>
+      <c r="J5" s="75"/>
+      <c r="K5" s="75"/>
+      <c r="L5" s="75"/>
+      <c r="M5" s="75"/>
+      <c r="N5" s="75"/>
+      <c r="O5" s="75"/>
       <c r="P5" s="75"/>
-      <c r="Q5" s="58"/>
-      <c r="R5" s="71" t="s">
+      <c r="Q5" s="76"/>
+      <c r="R5" s="58"/>
+      <c r="S5" s="72" t="s">
         <v>10</v>
       </c>
-      <c r="S5" s="71"/>
       <c r="T5" s="72"/>
-      <c r="Z5" s="1" t="s">
+      <c r="U5" s="73"/>
+      <c r="AA5" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="53" t="s">
         <v>12</v>
       </c>
@@ -1189,61 +1200,64 @@
         <v>8</v>
       </c>
       <c r="F6" s="54" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="G6" s="54" t="s">
+      <c r="H6" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="H6" s="54" t="s">
+      <c r="I6" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="I6" s="56" t="s">
+      <c r="J6" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="J6" s="54" t="s">
+      <c r="K6" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="K6" s="55" t="s">
+      <c r="L6" s="55" t="s">
         <v>17</v>
       </c>
-      <c r="L6" s="54" t="s">
+      <c r="M6" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="M6" s="54" t="s">
+      <c r="N6" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="N6" s="54" t="s">
+      <c r="O6" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="O6" s="54" t="s">
+      <c r="P6" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="P6" s="67" t="s">
+      <c r="Q6" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="Q6" s="54" t="s">
+      <c r="R6" s="54" t="s">
         <v>24</v>
       </c>
-      <c r="R6" s="54" t="s">
+      <c r="S6" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="S6" s="54" t="s">
+      <c r="T6" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="T6" s="57" t="s">
+      <c r="U6" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="W6" s="8" t="s">
+      <c r="X6" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="X6" s="8" t="s">
+      <c r="Y6" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="Z6" s="1" t="s">
+      <c r="AA6" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:26" s="15" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" s="15" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="16">
         <v>0</v>
       </c>
@@ -1256,7 +1270,7 @@
       <c r="E7" s="18">
         <v>3</v>
       </c>
-      <c r="F7" s="17">
+      <c r="F7" s="18">
         <v>4</v>
       </c>
       <c r="G7" s="17">
@@ -1280,90 +1294,94 @@
       <c r="M7" s="17">
         <v>11</v>
       </c>
-      <c r="N7" s="31">
+      <c r="N7" s="17">
         <v>12</v>
       </c>
-      <c r="O7" s="19">
+      <c r="O7" s="31">
         <v>13</v>
       </c>
-      <c r="P7" s="68">
+      <c r="P7" s="19">
         <v>14</v>
       </c>
-      <c r="Q7" s="19">
+      <c r="Q7" s="68">
+        <v>15</v>
+      </c>
+      <c r="R7" s="19">
         <v>14</v>
       </c>
-      <c r="R7" s="50">
-        <f>IF(ISBLANK(S7),0,ROUND((Q7-S7)*(P7/Q7),0))</f>
+      <c r="S7" s="50">
+        <f>IF(ISBLANK(T7),0,ROUND((R7-T7)*(Q7/R7),0))</f>
         <v>0</v>
       </c>
-      <c r="S7" s="23"/>
-      <c r="T7" s="49"/>
-      <c r="W7" s="15">
-        <f>R7/ROUND(P7,0)</f>
+      <c r="T7" s="23"/>
+      <c r="U7" s="49"/>
+      <c r="X7" s="15">
+        <f>S7/ROUND(Q7,0)</f>
         <v>0</v>
       </c>
-      <c r="X7" s="15">
-        <f>W7*I7</f>
+      <c r="Y7" s="15">
+        <f>X7*J7</f>
         <v>0</v>
       </c>
-      <c r="Z7" s="1" t="s">
+      <c r="AA7" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:27" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="B8" s="9"/>
       <c r="C8" s="10"/>
       <c r="D8" s="27"/>
       <c r="E8" s="12"/>
-      <c r="F8" s="11"/>
+      <c r="F8" s="12"/>
       <c r="G8" s="11"/>
       <c r="H8" s="11"/>
-      <c r="I8" s="29"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="25"/>
-      <c r="L8" s="11"/>
-      <c r="M8" s="14"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="29"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="25"/>
+      <c r="M8" s="11"/>
       <c r="N8" s="14"/>
       <c r="O8" s="14"/>
-      <c r="P8" s="69"/>
-      <c r="Q8" s="20"/>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="69"/>
       <c r="R8" s="20"/>
-      <c r="S8" s="21" t="str">
-        <f t="shared" ref="S8" si="0">CONCATENATE(C8," ",F8, " ",J8)</f>
+      <c r="S8" s="20"/>
+      <c r="T8" s="21" t="str">
+        <f t="shared" ref="T8" si="0">CONCATENATE(C8," ",G8, " ",K8)</f>
         <v xml:space="preserve">  </v>
       </c>
-      <c r="T8" s="22">
-        <f t="shared" ref="T8" si="1">G8</f>
+      <c r="U8" s="22">
+        <f t="shared" ref="U8" si="1">H8</f>
         <v>0</v>
       </c>
-      <c r="Z8" s="1" t="s">
+      <c r="AA8" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="S9" s="6"/>
-      <c r="Z9" s="1" t="s">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="T9" s="6"/>
+      <c r="AA9" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="S10" s="6"/>
-    </row>
-    <row r="12" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="F12" s="7"/>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="T10" s="6"/>
+    </row>
+    <row r="12" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
-      <c r="I12" s="30"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="26"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="30"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="R5:T5"/>
-    <mergeCell ref="B5:P5"/>
-    <mergeCell ref="B1:T1"/>
-    <mergeCell ref="B2:T2"/>
+    <mergeCell ref="S5:U5"/>
+    <mergeCell ref="B5:Q5"/>
+    <mergeCell ref="B1:U1"/>
+    <mergeCell ref="B2:U2"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1412,51 +1430,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="76" t="str">
-        <f>'STAFF LIST'!B1:T1</f>
+      <c r="B1" s="77" t="str">
+        <f>'STAFF LIST'!B1:U1</f>
         <v>713H CLAIMS FOR VENDOR NAME</v>
       </c>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="76"/>
-      <c r="H1" s="76"/>
-      <c r="I1" s="76"/>
-      <c r="J1" s="76"/>
-      <c r="K1" s="76"/>
-      <c r="L1" s="76"/>
-      <c r="M1" s="76"/>
-      <c r="N1" s="76"/>
-      <c r="O1" s="76"/>
-      <c r="P1" s="76"/>
-      <c r="Q1" s="76"/>
-      <c r="R1" s="76"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="77"/>
+      <c r="L1" s="77"/>
+      <c r="M1" s="77"/>
+      <c r="N1" s="77"/>
+      <c r="O1" s="77"/>
+      <c r="P1" s="77"/>
+      <c r="Q1" s="77"/>
+      <c r="R1" s="77"/>
       <c r="X1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:24" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="77" t="str">
-        <f>'STAFF LIST'!B2:T2</f>
+      <c r="B2" s="78" t="str">
+        <f>'STAFF LIST'!B2:U2</f>
         <v>Aug-16 to Sep-16</v>
       </c>
-      <c r="C2" s="77"/>
-      <c r="D2" s="77"/>
-      <c r="E2" s="77"/>
-      <c r="F2" s="77"/>
-      <c r="G2" s="77"/>
-      <c r="H2" s="77"/>
-      <c r="I2" s="77"/>
-      <c r="J2" s="77"/>
-      <c r="K2" s="77"/>
-      <c r="L2" s="77"/>
-      <c r="M2" s="77"/>
-      <c r="N2" s="77"/>
-      <c r="O2" s="77"/>
-      <c r="P2" s="77"/>
-      <c r="Q2" s="77"/>
-      <c r="R2" s="77"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="78"/>
+      <c r="K2" s="78"/>
+      <c r="L2" s="78"/>
+      <c r="M2" s="78"/>
+      <c r="N2" s="78"/>
+      <c r="O2" s="78"/>
+      <c r="P2" s="78"/>
+      <c r="Q2" s="78"/>
+      <c r="R2" s="78"/>
       <c r="X2" s="1" t="s">
         <v>15</v>
       </c>
@@ -1503,27 +1521,27 @@
       </c>
     </row>
     <row r="5" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="78" t="s">
+      <c r="B5" s="79" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="79"/>
-      <c r="D5" s="79"/>
-      <c r="E5" s="79"/>
-      <c r="F5" s="79"/>
-      <c r="G5" s="79"/>
-      <c r="H5" s="79"/>
-      <c r="I5" s="79"/>
-      <c r="J5" s="79"/>
-      <c r="K5" s="79"/>
-      <c r="L5" s="79"/>
-      <c r="M5" s="79"/>
-      <c r="N5" s="79"/>
-      <c r="O5" s="79"/>
-      <c r="P5" s="80" t="s">
+      <c r="C5" s="80"/>
+      <c r="D5" s="80"/>
+      <c r="E5" s="80"/>
+      <c r="F5" s="80"/>
+      <c r="G5" s="80"/>
+      <c r="H5" s="80"/>
+      <c r="I5" s="80"/>
+      <c r="J5" s="80"/>
+      <c r="K5" s="80"/>
+      <c r="L5" s="80"/>
+      <c r="M5" s="80"/>
+      <c r="N5" s="80"/>
+      <c r="O5" s="80"/>
+      <c r="P5" s="81" t="s">
         <v>10</v>
       </c>
-      <c r="Q5" s="80"/>
-      <c r="R5" s="81"/>
+      <c r="Q5" s="81"/>
+      <c r="R5" s="82"/>
       <c r="X5" s="1" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
added additional % column to the form
</commit_message>
<xml_diff>
--- a/creator/forms_xlsx/DATASHEET.xlsx
+++ b/creator/forms_xlsx/DATASHEET.xlsx
@@ -16,8 +16,8 @@
     <sheet name="MISMATCH" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">MISMATCH!$B$6:$R$6</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'STAFF LIST'!$B$6:$U$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">MISMATCH!$B$6:$S$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'STAFF LIST'!$B$6:$V$6</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="28">
   <si>
     <t>ResID</t>
   </si>
@@ -124,6 +124,9 @@
   </si>
   <si>
     <t>Director</t>
+  </si>
+  <si>
+    <t>Additional %</t>
   </si>
 </sst>
 </file>
@@ -503,7 +506,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -701,6 +704,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1022,10 +1028,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AA12"/>
+  <dimension ref="A1:AB12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="V7" sqref="V7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1037,80 +1043,82 @@
     <col min="5" max="6" width="39.5703125" style="1" customWidth="1"/>
     <col min="7" max="7" width="7.5703125" style="1" customWidth="1"/>
     <col min="8" max="9" width="12" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" style="28" customWidth="1"/>
-    <col min="11" max="11" width="17.28515625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="44.140625" style="24" customWidth="1"/>
-    <col min="13" max="13" width="21.42578125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="13.42578125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="17.5703125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="15" style="1" customWidth="1"/>
-    <col min="17" max="17" width="17.85546875" style="70" customWidth="1"/>
-    <col min="18" max="18" width="17.85546875" style="1" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="15.28515625" style="1" customWidth="1"/>
-    <col min="20" max="20" width="8.5703125" style="1" customWidth="1"/>
-    <col min="21" max="21" width="40" style="1" customWidth="1"/>
-    <col min="22" max="23" width="9.140625" style="1"/>
-    <col min="24" max="24" width="11" style="1" customWidth="1"/>
-    <col min="25" max="26" width="9.140625" style="1" customWidth="1"/>
-    <col min="27" max="27" width="9.140625" style="1" hidden="1" customWidth="1"/>
-    <col min="28" max="16384" width="9.140625" style="1"/>
+    <col min="10" max="11" width="12.5703125" style="28" customWidth="1"/>
+    <col min="12" max="12" width="17.28515625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="44.140625" style="24" customWidth="1"/>
+    <col min="14" max="14" width="21.42578125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="13.42578125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="17.5703125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="15" style="1" customWidth="1"/>
+    <col min="18" max="18" width="17.85546875" style="70" customWidth="1"/>
+    <col min="19" max="19" width="17.85546875" style="1" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="15.28515625" style="1" customWidth="1"/>
+    <col min="21" max="21" width="8.5703125" style="1" customWidth="1"/>
+    <col min="22" max="22" width="40" style="1" customWidth="1"/>
+    <col min="23" max="24" width="9.140625" style="1"/>
+    <col min="25" max="25" width="11" style="1" customWidth="1"/>
+    <col min="26" max="27" width="9.140625" style="1" customWidth="1"/>
+    <col min="28" max="28" width="9.140625" style="1" hidden="1" customWidth="1"/>
+    <col min="29" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="77" t="s">
+    <row r="1" spans="1:28" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
-      <c r="J1" s="77"/>
-      <c r="K1" s="77"/>
-      <c r="L1" s="77"/>
-      <c r="M1" s="77"/>
-      <c r="N1" s="77"/>
-      <c r="O1" s="77"/>
-      <c r="P1" s="77"/>
-      <c r="Q1" s="77"/>
-      <c r="R1" s="77"/>
-      <c r="S1" s="77"/>
-      <c r="T1" s="77"/>
-      <c r="U1" s="77"/>
-      <c r="AA1" s="1" t="s">
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="78"/>
+      <c r="K1" s="78"/>
+      <c r="L1" s="78"/>
+      <c r="M1" s="78"/>
+      <c r="N1" s="78"/>
+      <c r="O1" s="78"/>
+      <c r="P1" s="78"/>
+      <c r="Q1" s="78"/>
+      <c r="R1" s="78"/>
+      <c r="S1" s="78"/>
+      <c r="T1" s="78"/>
+      <c r="U1" s="78"/>
+      <c r="V1" s="78"/>
+      <c r="AB1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="78" t="s">
+    <row r="2" spans="1:28" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="79" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78"/>
-      <c r="I2" s="78"/>
-      <c r="J2" s="78"/>
-      <c r="K2" s="78"/>
-      <c r="L2" s="78"/>
-      <c r="M2" s="78"/>
-      <c r="N2" s="78"/>
-      <c r="O2" s="78"/>
-      <c r="P2" s="78"/>
-      <c r="Q2" s="78"/>
-      <c r="R2" s="78"/>
-      <c r="S2" s="78"/>
-      <c r="T2" s="78"/>
-      <c r="U2" s="78"/>
-      <c r="AA2" s="1" t="s">
+      <c r="C2" s="79"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="79"/>
+      <c r="J2" s="79"/>
+      <c r="K2" s="79"/>
+      <c r="L2" s="79"/>
+      <c r="M2" s="79"/>
+      <c r="N2" s="79"/>
+      <c r="O2" s="79"/>
+      <c r="P2" s="79"/>
+      <c r="Q2" s="79"/>
+      <c r="R2" s="79"/>
+      <c r="S2" s="79"/>
+      <c r="T2" s="79"/>
+      <c r="U2" s="79"/>
+      <c r="V2" s="79"/>
+      <c r="AB2" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:27" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="51"/>
       <c r="C3" s="51"/>
       <c r="D3" s="51"/>
@@ -1120,19 +1128,20 @@
       <c r="H3" s="51"/>
       <c r="I3" s="51"/>
       <c r="J3" s="51"/>
-      <c r="K3" s="51"/>
+      <c r="K3" s="72"/>
       <c r="L3" s="51"/>
       <c r="M3" s="51"/>
       <c r="N3" s="51"/>
       <c r="O3" s="51"/>
       <c r="P3" s="51"/>
-      <c r="Q3" s="65"/>
-      <c r="R3" s="51"/>
+      <c r="Q3" s="51"/>
+      <c r="R3" s="65"/>
       <c r="S3" s="51"/>
       <c r="T3" s="51"/>
       <c r="U3" s="51"/>
-    </row>
-    <row r="4" spans="1:27" ht="33" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V3" s="51"/>
+    </row>
+    <row r="4" spans="1:28" ht="33" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="59"/>
       <c r="C4" s="60"/>
       <c r="D4" s="61"/>
@@ -1142,51 +1151,53 @@
       <c r="H4" s="60"/>
       <c r="I4" s="60"/>
       <c r="J4" s="62"/>
-      <c r="K4" s="60"/>
-      <c r="L4" s="61"/>
-      <c r="M4" s="60"/>
+      <c r="K4" s="62"/>
+      <c r="L4" s="60"/>
+      <c r="M4" s="61"/>
       <c r="N4" s="60"/>
       <c r="O4" s="60"/>
       <c r="P4" s="60"/>
-      <c r="Q4" s="66"/>
-      <c r="R4" s="60"/>
-      <c r="S4" s="63"/>
-      <c r="T4" s="60"/>
-      <c r="U4" s="64"/>
-      <c r="AA4" s="1" t="s">
+      <c r="Q4" s="60"/>
+      <c r="R4" s="66"/>
+      <c r="S4" s="60"/>
+      <c r="T4" s="63"/>
+      <c r="U4" s="60"/>
+      <c r="V4" s="64"/>
+      <c r="AB4" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:27" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="74" t="s">
+    <row r="5" spans="1:28" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="75"/>
-      <c r="D5" s="75"/>
-      <c r="E5" s="75"/>
-      <c r="F5" s="75"/>
-      <c r="G5" s="75"/>
-      <c r="H5" s="75"/>
-      <c r="I5" s="75"/>
-      <c r="J5" s="75"/>
-      <c r="K5" s="75"/>
-      <c r="L5" s="75"/>
-      <c r="M5" s="75"/>
-      <c r="N5" s="75"/>
-      <c r="O5" s="75"/>
-      <c r="P5" s="75"/>
+      <c r="C5" s="76"/>
+      <c r="D5" s="76"/>
+      <c r="E5" s="76"/>
+      <c r="F5" s="76"/>
+      <c r="G5" s="76"/>
+      <c r="H5" s="76"/>
+      <c r="I5" s="76"/>
+      <c r="J5" s="76"/>
+      <c r="K5" s="76"/>
+      <c r="L5" s="76"/>
+      <c r="M5" s="76"/>
+      <c r="N5" s="76"/>
+      <c r="O5" s="76"/>
+      <c r="P5" s="76"/>
       <c r="Q5" s="76"/>
-      <c r="R5" s="58"/>
-      <c r="S5" s="72" t="s">
+      <c r="R5" s="77"/>
+      <c r="S5" s="58"/>
+      <c r="T5" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="T5" s="72"/>
       <c r="U5" s="73"/>
-      <c r="AA5" s="1" t="s">
+      <c r="V5" s="74"/>
+      <c r="AB5" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:27" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="53" t="s">
         <v>12</v>
       </c>
@@ -1214,50 +1225,53 @@
       <c r="J6" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="K6" s="54" t="s">
+      <c r="K6" s="56" t="s">
+        <v>27</v>
+      </c>
+      <c r="L6" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="L6" s="55" t="s">
+      <c r="M6" s="55" t="s">
         <v>17</v>
       </c>
-      <c r="M6" s="54" t="s">
+      <c r="N6" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="N6" s="54" t="s">
+      <c r="O6" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="O6" s="54" t="s">
+      <c r="P6" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="P6" s="54" t="s">
+      <c r="Q6" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="Q6" s="67" t="s">
+      <c r="R6" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="R6" s="54" t="s">
+      <c r="S6" s="54" t="s">
         <v>24</v>
       </c>
-      <c r="S6" s="54" t="s">
+      <c r="T6" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="T6" s="54" t="s">
+      <c r="U6" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="U6" s="57" t="s">
+      <c r="V6" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="X6" s="8" t="s">
+      <c r="Y6" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="Y6" s="8" t="s">
+      <c r="Z6" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="AA6" s="1" t="s">
+      <c r="AB6" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:27" s="15" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" s="15" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="16">
         <v>0</v>
       </c>
@@ -1297,37 +1311,40 @@
       <c r="N7" s="17">
         <v>12</v>
       </c>
-      <c r="O7" s="31">
+      <c r="O7" s="17">
         <v>13</v>
       </c>
-      <c r="P7" s="19">
+      <c r="P7" s="31">
         <v>14</v>
       </c>
-      <c r="Q7" s="68">
+      <c r="Q7" s="19">
         <v>15</v>
       </c>
-      <c r="R7" s="19">
+      <c r="R7" s="68">
+        <v>16</v>
+      </c>
+      <c r="S7" s="19">
         <v>14</v>
       </c>
-      <c r="S7" s="50">
-        <f>IF(ISBLANK(T7),0,ROUND((R7-T7)*(Q7/R7),0))</f>
+      <c r="T7" s="50">
+        <f>IF(ISBLANK(U7),0,ROUND((S7-U7)*(R7/S7),0))</f>
         <v>0</v>
       </c>
-      <c r="T7" s="23"/>
-      <c r="U7" s="49"/>
-      <c r="X7" s="15">
-        <f>S7/ROUND(Q7,0)</f>
+      <c r="U7" s="23"/>
+      <c r="V7" s="49"/>
+      <c r="Y7" s="15">
+        <f>T7/ROUND(R7,0)</f>
         <v>0</v>
       </c>
-      <c r="Y7" s="15">
-        <f>X7*J7</f>
+      <c r="Z7" s="15">
+        <f>Y7*J7</f>
         <v>0</v>
       </c>
-      <c r="AA7" s="1" t="s">
+      <c r="AB7" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:27" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="B8" s="9"/>
       <c r="C8" s="10"/>
@@ -1338,50 +1355,52 @@
       <c r="H8" s="11"/>
       <c r="I8" s="11"/>
       <c r="J8" s="29"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="25"/>
-      <c r="M8" s="11"/>
-      <c r="N8" s="14"/>
+      <c r="K8" s="29"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="25"/>
+      <c r="N8" s="11"/>
       <c r="O8" s="14"/>
       <c r="P8" s="14"/>
-      <c r="Q8" s="69"/>
-      <c r="R8" s="20"/>
+      <c r="Q8" s="14"/>
+      <c r="R8" s="69"/>
       <c r="S8" s="20"/>
-      <c r="T8" s="21" t="str">
-        <f t="shared" ref="T8" si="0">CONCATENATE(C8," ",G8, " ",K8)</f>
+      <c r="T8" s="20"/>
+      <c r="U8" s="21" t="str">
+        <f>CONCATENATE(C8," ",G8, " ",L8)</f>
         <v xml:space="preserve">  </v>
       </c>
-      <c r="U8" s="22">
-        <f t="shared" ref="U8" si="1">H8</f>
+      <c r="V8" s="22">
+        <f t="shared" ref="V8" si="0">H8</f>
         <v>0</v>
       </c>
-      <c r="AA8" s="1" t="s">
+      <c r="AB8" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="T9" s="6"/>
-      <c r="AA9" s="1" t="s">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="U9" s="6"/>
+      <c r="AB9" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="T10" s="6"/>
-    </row>
-    <row r="12" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="U10" s="6"/>
+    </row>
+    <row r="12" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
       <c r="J12" s="30"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="26"/>
+      <c r="K12" s="30"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="S5:U5"/>
-    <mergeCell ref="B5:Q5"/>
-    <mergeCell ref="B1:U1"/>
-    <mergeCell ref="B2:U2"/>
+    <mergeCell ref="T5:V5"/>
+    <mergeCell ref="B5:R5"/>
+    <mergeCell ref="B1:V1"/>
+    <mergeCell ref="B2:V2"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1394,13 +1413,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X12"/>
+  <dimension ref="A1:Y12"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="10" ySplit="6" topLeftCell="K7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="11" ySplit="6" topLeftCell="L7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="G40" sqref="G40"/>
+      <selection pane="bottomRight" activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1412,74 +1431,76 @@
     <col min="5" max="5" width="29.7109375" style="45" customWidth="1"/>
     <col min="6" max="6" width="7.5703125" style="45" customWidth="1"/>
     <col min="7" max="7" width="10" style="45" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" style="45" customWidth="1"/>
-    <col min="9" max="9" width="17.28515625" style="45" customWidth="1"/>
-    <col min="10" max="10" width="29.28515625" style="45" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" style="45" customWidth="1"/>
-    <col min="12" max="12" width="17.140625" style="45" customWidth="1"/>
-    <col min="13" max="13" width="19.42578125" style="45" customWidth="1"/>
-    <col min="14" max="14" width="15" style="45" customWidth="1"/>
-    <col min="15" max="15" width="22.28515625" style="45" customWidth="1"/>
-    <col min="16" max="16" width="15.28515625" style="45" customWidth="1"/>
-    <col min="17" max="17" width="8.5703125" style="45" customWidth="1"/>
-    <col min="18" max="18" width="40" style="45" customWidth="1"/>
-    <col min="19" max="20" width="9.140625" style="1"/>
-    <col min="21" max="21" width="11" style="1" customWidth="1"/>
-    <col min="22" max="24" width="9.140625" style="1" customWidth="1"/>
-    <col min="25" max="16384" width="9.140625" style="1"/>
+    <col min="8" max="9" width="12.5703125" style="45" customWidth="1"/>
+    <col min="10" max="10" width="17.28515625" style="45" customWidth="1"/>
+    <col min="11" max="11" width="29.28515625" style="45" customWidth="1"/>
+    <col min="12" max="12" width="12.7109375" style="45" customWidth="1"/>
+    <col min="13" max="13" width="17.140625" style="45" customWidth="1"/>
+    <col min="14" max="14" width="19.42578125" style="45" customWidth="1"/>
+    <col min="15" max="15" width="15" style="45" customWidth="1"/>
+    <col min="16" max="16" width="22.28515625" style="45" customWidth="1"/>
+    <col min="17" max="17" width="15.28515625" style="45" customWidth="1"/>
+    <col min="18" max="18" width="8.5703125" style="45" customWidth="1"/>
+    <col min="19" max="19" width="40" style="45" customWidth="1"/>
+    <col min="20" max="21" width="9.140625" style="1"/>
+    <col min="22" max="22" width="11" style="1" customWidth="1"/>
+    <col min="23" max="25" width="9.140625" style="1" customWidth="1"/>
+    <col min="26" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="77" t="str">
-        <f>'STAFF LIST'!B1:U1</f>
+    <row r="1" spans="1:25" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="78" t="str">
+        <f>'STAFF LIST'!B1:V1</f>
         <v>713H CLAIMS FOR VENDOR NAME</v>
       </c>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
-      <c r="J1" s="77"/>
-      <c r="K1" s="77"/>
-      <c r="L1" s="77"/>
-      <c r="M1" s="77"/>
-      <c r="N1" s="77"/>
-      <c r="O1" s="77"/>
-      <c r="P1" s="77"/>
-      <c r="Q1" s="77"/>
-      <c r="R1" s="77"/>
-      <c r="X1" s="1" t="s">
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="78"/>
+      <c r="K1" s="78"/>
+      <c r="L1" s="78"/>
+      <c r="M1" s="78"/>
+      <c r="N1" s="78"/>
+      <c r="O1" s="78"/>
+      <c r="P1" s="78"/>
+      <c r="Q1" s="78"/>
+      <c r="R1" s="78"/>
+      <c r="S1" s="78"/>
+      <c r="Y1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="78" t="str">
-        <f>'STAFF LIST'!B2:U2</f>
+    <row r="2" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="79" t="str">
+        <f>'STAFF LIST'!B2:V2</f>
         <v>Aug-16 to Sep-16</v>
       </c>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78"/>
-      <c r="I2" s="78"/>
-      <c r="J2" s="78"/>
-      <c r="K2" s="78"/>
-      <c r="L2" s="78"/>
-      <c r="M2" s="78"/>
-      <c r="N2" s="78"/>
-      <c r="O2" s="78"/>
-      <c r="P2" s="78"/>
-      <c r="Q2" s="78"/>
-      <c r="R2" s="78"/>
-      <c r="X2" s="1" t="s">
+      <c r="C2" s="79"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="79"/>
+      <c r="J2" s="79"/>
+      <c r="K2" s="79"/>
+      <c r="L2" s="79"/>
+      <c r="M2" s="79"/>
+      <c r="N2" s="79"/>
+      <c r="O2" s="79"/>
+      <c r="P2" s="79"/>
+      <c r="Q2" s="79"/>
+      <c r="R2" s="79"/>
+      <c r="S2" s="79"/>
+      <c r="Y2" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="52"/>
       <c r="C3" s="52"/>
       <c r="D3" s="52"/>
@@ -1487,7 +1508,7 @@
       <c r="F3" s="52"/>
       <c r="G3" s="52"/>
       <c r="H3" s="52"/>
-      <c r="I3" s="52"/>
+      <c r="I3" s="72"/>
       <c r="J3" s="52"/>
       <c r="K3" s="52"/>
       <c r="L3" s="52"/>
@@ -1497,8 +1518,9 @@
       <c r="P3" s="52"/>
       <c r="Q3" s="52"/>
       <c r="R3" s="52"/>
-    </row>
-    <row r="4" spans="1:24" ht="33" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S3" s="52"/>
+    </row>
+    <row r="4" spans="1:25" ht="33" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -1513,40 +1535,42 @@
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="2"/>
       <c r="R4" s="1"/>
-      <c r="X4" s="1" t="s">
+      <c r="S4" s="1"/>
+      <c r="Y4" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="79" t="s">
+    <row r="5" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="80" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="80"/>
-      <c r="D5" s="80"/>
-      <c r="E5" s="80"/>
-      <c r="F5" s="80"/>
-      <c r="G5" s="80"/>
-      <c r="H5" s="80"/>
-      <c r="I5" s="80"/>
-      <c r="J5" s="80"/>
-      <c r="K5" s="80"/>
-      <c r="L5" s="80"/>
-      <c r="M5" s="80"/>
-      <c r="N5" s="80"/>
-      <c r="O5" s="80"/>
-      <c r="P5" s="81" t="s">
+      <c r="C5" s="81"/>
+      <c r="D5" s="81"/>
+      <c r="E5" s="81"/>
+      <c r="F5" s="81"/>
+      <c r="G5" s="81"/>
+      <c r="H5" s="81"/>
+      <c r="I5" s="81"/>
+      <c r="J5" s="81"/>
+      <c r="K5" s="81"/>
+      <c r="L5" s="81"/>
+      <c r="M5" s="81"/>
+      <c r="N5" s="81"/>
+      <c r="O5" s="81"/>
+      <c r="P5" s="81"/>
+      <c r="Q5" s="82" t="s">
         <v>10</v>
       </c>
-      <c r="Q5" s="81"/>
       <c r="R5" s="82"/>
-      <c r="X5" s="1" t="s">
+      <c r="S5" s="83"/>
+      <c r="Y5" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:24" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>12</v>
       </c>
@@ -1569,46 +1593,49 @@
         <v>16</v>
       </c>
       <c r="I6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="J6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="J6" s="4" t="s">
+      <c r="K6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="K6" s="4" t="s">
+      <c r="L6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="L6" s="4" t="s">
+      <c r="M6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="M6" s="4" t="s">
+      <c r="N6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="N6" s="4" t="s">
+      <c r="O6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="O6" s="4" t="s">
+      <c r="P6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="P6" s="4" t="s">
+      <c r="Q6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="Q6" s="4" t="s">
+      <c r="R6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="R6" s="8" t="s">
+      <c r="S6" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="U6" s="8" t="s">
+      <c r="V6" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="V6" s="8" t="s">
+      <c r="W6" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="X6" s="1" t="s">
+      <c r="Y6" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:24" s="15" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" s="15" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="32"/>
       <c r="C7" s="33"/>
       <c r="D7" s="33"/>
@@ -1623,22 +1650,23 @@
       <c r="M7" s="33"/>
       <c r="N7" s="33"/>
       <c r="O7" s="33"/>
-      <c r="P7" s="48"/>
+      <c r="P7" s="33"/>
       <c r="Q7" s="48"/>
-      <c r="R7" s="35"/>
-      <c r="U7" s="15" t="e">
-        <f>P7/O7</f>
+      <c r="R7" s="48"/>
+      <c r="S7" s="35"/>
+      <c r="V7" s="15" t="e">
+        <f>Q7/P7</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="V7" s="15" t="e">
-        <f>U7*H7</f>
+      <c r="W7" s="15" t="e">
+        <f>V7*H7</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="X7" s="1" t="s">
+      <c r="Y7" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:24" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:25" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="B8" s="36"/>
       <c r="C8" s="37"/>
@@ -1647,48 +1675,50 @@
       <c r="F8" s="38"/>
       <c r="G8" s="38"/>
       <c r="H8" s="38"/>
-      <c r="I8" s="40"/>
+      <c r="I8" s="38"/>
       <c r="J8" s="40"/>
-      <c r="K8" s="38"/>
-      <c r="L8" s="41"/>
+      <c r="K8" s="40"/>
+      <c r="L8" s="38"/>
       <c r="M8" s="41"/>
       <c r="N8" s="41"/>
-      <c r="O8" s="42"/>
+      <c r="O8" s="41"/>
       <c r="P8" s="42"/>
-      <c r="Q8" s="43" t="str">
-        <f t="shared" ref="Q8" si="0">CONCATENATE(C8," ",F8, " ",I8)</f>
+      <c r="Q8" s="42"/>
+      <c r="R8" s="43" t="str">
+        <f t="shared" ref="R8" si="0">CONCATENATE(C8," ",F8, " ",J8)</f>
         <v xml:space="preserve">  </v>
       </c>
-      <c r="R8" s="44">
-        <f t="shared" ref="R8" si="1">G8</f>
+      <c r="S8" s="44">
+        <f t="shared" ref="S8" si="1">G8</f>
         <v>0</v>
       </c>
-      <c r="X8" s="1" t="s">
+      <c r="Y8" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="Q9" s="46"/>
-      <c r="X9" s="1" t="s">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="R9" s="46"/>
+      <c r="Y9" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="Q10" s="46"/>
-    </row>
-    <row r="12" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="R10" s="46"/>
+    </row>
+    <row r="12" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="F12" s="47"/>
       <c r="G12" s="47"/>
       <c r="H12" s="47"/>
       <c r="I12" s="47"/>
       <c r="J12" s="47"/>
+      <c r="K12" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="B1:R1"/>
-    <mergeCell ref="B2:R2"/>
-    <mergeCell ref="B5:O5"/>
-    <mergeCell ref="P5:R5"/>
+    <mergeCell ref="B1:S1"/>
+    <mergeCell ref="B2:S2"/>
+    <mergeCell ref="B5:P5"/>
+    <mergeCell ref="Q5:S5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added new fields to excel form
</commit_message>
<xml_diff>
--- a/creator/forms_xlsx/DATASHEET.xlsx
+++ b/creator/forms_xlsx/DATASHEET.xlsx
@@ -17,7 +17,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">MISMATCH!$B$6:$S$6</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'STAFF LIST'!$B$6:$V$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'STAFF LIST'!$B$6:$W$6</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="29">
   <si>
     <t>ResID</t>
   </si>
@@ -127,6 +127,9 @@
   </si>
   <si>
     <t>Additional %</t>
+  </si>
+  <si>
+    <t>Unit Rate</t>
   </si>
 </sst>
 </file>
@@ -506,7 +509,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -704,6 +707,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1028,10 +1034,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AB12"/>
+  <dimension ref="A1:AD12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1042,84 +1048,86 @@
     <col min="4" max="4" width="15.140625" style="24" customWidth="1"/>
     <col min="5" max="6" width="39.5703125" style="1" customWidth="1"/>
     <col min="7" max="7" width="7.5703125" style="1" customWidth="1"/>
-    <col min="8" max="9" width="12" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" style="28" customWidth="1"/>
-    <col min="11" max="11" width="12.5703125" style="28" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="17.28515625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="44.140625" style="24" customWidth="1"/>
-    <col min="14" max="14" width="21.42578125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="13.42578125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="17.5703125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="15" style="1" customWidth="1"/>
-    <col min="18" max="18" width="17.85546875" style="70" customWidth="1"/>
-    <col min="19" max="19" width="17.85546875" style="1" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="15.28515625" style="1" customWidth="1"/>
-    <col min="21" max="21" width="8.5703125" style="1" customWidth="1"/>
-    <col min="22" max="22" width="40" style="1" customWidth="1"/>
-    <col min="23" max="24" width="9.140625" style="1"/>
-    <col min="25" max="25" width="11" style="1" customWidth="1"/>
-    <col min="26" max="27" width="9.140625" style="1" customWidth="1"/>
-    <col min="28" max="28" width="9.140625" style="1" hidden="1" customWidth="1"/>
-    <col min="29" max="16384" width="9.140625" style="1"/>
+    <col min="8" max="10" width="12" style="1" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="12.5703125" style="28" customWidth="1"/>
+    <col min="13" max="13" width="17.28515625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="44.140625" style="24" customWidth="1"/>
+    <col min="15" max="15" width="21.42578125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="13.42578125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="17.5703125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="15" style="1" customWidth="1"/>
+    <col min="19" max="19" width="17.85546875" style="70" customWidth="1"/>
+    <col min="20" max="20" width="17.85546875" style="1" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="15.28515625" style="1" customWidth="1"/>
+    <col min="22" max="22" width="8.5703125" style="1" customWidth="1"/>
+    <col min="23" max="23" width="40" style="1" customWidth="1"/>
+    <col min="24" max="25" width="9.140625" style="1"/>
+    <col min="26" max="26" width="11" style="1" customWidth="1"/>
+    <col min="27" max="28" width="9.140625" style="1" customWidth="1"/>
+    <col min="29" max="29" width="9.140625" style="1" hidden="1" customWidth="1"/>
+    <col min="30" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="78" t="s">
+    <row r="1" spans="1:29" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="79" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="78"/>
-      <c r="I1" s="78"/>
-      <c r="J1" s="78"/>
-      <c r="K1" s="78"/>
-      <c r="L1" s="78"/>
-      <c r="M1" s="78"/>
-      <c r="N1" s="78"/>
-      <c r="O1" s="78"/>
-      <c r="P1" s="78"/>
-      <c r="Q1" s="78"/>
-      <c r="R1" s="78"/>
-      <c r="S1" s="78"/>
-      <c r="T1" s="78"/>
-      <c r="U1" s="78"/>
-      <c r="V1" s="78"/>
-      <c r="AB1" s="1" t="s">
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="79"/>
+      <c r="J1" s="79"/>
+      <c r="K1" s="79"/>
+      <c r="L1" s="79"/>
+      <c r="M1" s="79"/>
+      <c r="N1" s="79"/>
+      <c r="O1" s="79"/>
+      <c r="P1" s="79"/>
+      <c r="Q1" s="79"/>
+      <c r="R1" s="79"/>
+      <c r="S1" s="79"/>
+      <c r="T1" s="79"/>
+      <c r="U1" s="79"/>
+      <c r="V1" s="79"/>
+      <c r="W1" s="79"/>
+      <c r="AC1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:28" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="79" t="s">
+    <row r="2" spans="1:29" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="80" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="79"/>
-      <c r="D2" s="79"/>
-      <c r="E2" s="79"/>
-      <c r="F2" s="79"/>
-      <c r="G2" s="79"/>
-      <c r="H2" s="79"/>
-      <c r="I2" s="79"/>
-      <c r="J2" s="79"/>
-      <c r="K2" s="79"/>
-      <c r="L2" s="79"/>
-      <c r="M2" s="79"/>
-      <c r="N2" s="79"/>
-      <c r="O2" s="79"/>
-      <c r="P2" s="79"/>
-      <c r="Q2" s="79"/>
-      <c r="R2" s="79"/>
-      <c r="S2" s="79"/>
-      <c r="T2" s="79"/>
-      <c r="U2" s="79"/>
-      <c r="V2" s="79"/>
-      <c r="AB2" s="1" t="s">
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
+      <c r="J2" s="80"/>
+      <c r="K2" s="80"/>
+      <c r="L2" s="80"/>
+      <c r="M2" s="80"/>
+      <c r="N2" s="80"/>
+      <c r="O2" s="80"/>
+      <c r="P2" s="80"/>
+      <c r="Q2" s="80"/>
+      <c r="R2" s="80"/>
+      <c r="S2" s="80"/>
+      <c r="T2" s="80"/>
+      <c r="U2" s="80"/>
+      <c r="V2" s="80"/>
+      <c r="W2" s="80"/>
+      <c r="AC2" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:28" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:29" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="51"/>
       <c r="C3" s="51"/>
       <c r="D3" s="51"/>
@@ -1128,21 +1136,22 @@
       <c r="G3" s="51"/>
       <c r="H3" s="51"/>
       <c r="I3" s="51"/>
-      <c r="J3" s="51"/>
-      <c r="K3" s="72"/>
+      <c r="J3" s="73"/>
+      <c r="K3" s="73"/>
       <c r="L3" s="51"/>
       <c r="M3" s="51"/>
       <c r="N3" s="51"/>
       <c r="O3" s="51"/>
       <c r="P3" s="51"/>
       <c r="Q3" s="51"/>
-      <c r="R3" s="65"/>
-      <c r="S3" s="51"/>
+      <c r="R3" s="51"/>
+      <c r="S3" s="65"/>
       <c r="T3" s="51"/>
       <c r="U3" s="51"/>
       <c r="V3" s="51"/>
-    </row>
-    <row r="4" spans="1:28" ht="33" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="W3" s="51"/>
+    </row>
+    <row r="4" spans="1:29" ht="33" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="59"/>
       <c r="C4" s="60"/>
       <c r="D4" s="61"/>
@@ -1151,54 +1160,56 @@
       <c r="G4" s="60"/>
       <c r="H4" s="60"/>
       <c r="I4" s="60"/>
-      <c r="J4" s="62"/>
-      <c r="K4" s="62"/>
-      <c r="L4" s="60"/>
-      <c r="M4" s="61"/>
-      <c r="N4" s="60"/>
+      <c r="J4" s="60"/>
+      <c r="K4" s="60"/>
+      <c r="L4" s="62"/>
+      <c r="M4" s="60"/>
+      <c r="N4" s="61"/>
       <c r="O4" s="60"/>
       <c r="P4" s="60"/>
       <c r="Q4" s="60"/>
-      <c r="R4" s="66"/>
-      <c r="S4" s="60"/>
-      <c r="T4" s="63"/>
-      <c r="U4" s="60"/>
-      <c r="V4" s="64"/>
-      <c r="AB4" s="1" t="s">
+      <c r="R4" s="60"/>
+      <c r="S4" s="66"/>
+      <c r="T4" s="60"/>
+      <c r="U4" s="63"/>
+      <c r="V4" s="60"/>
+      <c r="W4" s="64"/>
+      <c r="AC4" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:28" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="75" t="s">
+    <row r="5" spans="1:29" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="76" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="76"/>
-      <c r="D5" s="76"/>
-      <c r="E5" s="76"/>
-      <c r="F5" s="76"/>
-      <c r="G5" s="76"/>
-      <c r="H5" s="76"/>
-      <c r="I5" s="76"/>
-      <c r="J5" s="76"/>
-      <c r="K5" s="76"/>
-      <c r="L5" s="76"/>
-      <c r="M5" s="76"/>
-      <c r="N5" s="76"/>
-      <c r="O5" s="76"/>
-      <c r="P5" s="76"/>
-      <c r="Q5" s="76"/>
+      <c r="C5" s="77"/>
+      <c r="D5" s="77"/>
+      <c r="E5" s="77"/>
+      <c r="F5" s="77"/>
+      <c r="G5" s="77"/>
+      <c r="H5" s="77"/>
+      <c r="I5" s="77"/>
+      <c r="J5" s="77"/>
+      <c r="K5" s="77"/>
+      <c r="L5" s="77"/>
+      <c r="M5" s="77"/>
+      <c r="N5" s="77"/>
+      <c r="O5" s="77"/>
+      <c r="P5" s="77"/>
+      <c r="Q5" s="77"/>
       <c r="R5" s="77"/>
-      <c r="S5" s="58"/>
-      <c r="T5" s="73" t="s">
+      <c r="S5" s="78"/>
+      <c r="T5" s="58"/>
+      <c r="U5" s="74" t="s">
         <v>10</v>
       </c>
-      <c r="U5" s="73"/>
       <c r="V5" s="74"/>
-      <c r="AB5" s="1" t="s">
+      <c r="W5" s="75"/>
+      <c r="AC5" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:28" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="53" t="s">
         <v>12</v>
       </c>
@@ -1223,56 +1234,59 @@
       <c r="I6" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="J6" s="56" t="s">
-        <v>16</v>
+      <c r="J6" s="54" t="s">
+        <v>28</v>
       </c>
       <c r="K6" s="56" t="s">
         <v>27</v>
       </c>
-      <c r="L6" s="54" t="s">
+      <c r="L6" s="56" t="s">
+        <v>16</v>
+      </c>
+      <c r="M6" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="M6" s="55" t="s">
+      <c r="N6" s="55" t="s">
         <v>17</v>
       </c>
-      <c r="N6" s="54" t="s">
+      <c r="O6" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="O6" s="54" t="s">
+      <c r="P6" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="P6" s="54" t="s">
+      <c r="Q6" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="Q6" s="54" t="s">
+      <c r="R6" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="R6" s="67" t="s">
+      <c r="S6" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="S6" s="54" t="s">
+      <c r="T6" s="54" t="s">
         <v>24</v>
       </c>
-      <c r="T6" s="54" t="s">
+      <c r="U6" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="U6" s="54" t="s">
+      <c r="V6" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="V6" s="57" t="s">
+      <c r="W6" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="Y6" s="8" t="s">
+      <c r="Z6" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="Z6" s="8" t="s">
+      <c r="AA6" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="AB6" s="1" t="s">
+      <c r="AC6" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:28" s="15" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" s="15" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="16">
         <v>0</v>
       </c>
@@ -1315,37 +1329,40 @@
       <c r="O7" s="17">
         <v>13</v>
       </c>
-      <c r="P7" s="31">
+      <c r="P7" s="17">
         <v>14</v>
       </c>
-      <c r="Q7" s="19">
+      <c r="Q7" s="31">
         <v>15</v>
       </c>
-      <c r="R7" s="68">
+      <c r="R7" s="19">
         <v>16</v>
       </c>
-      <c r="S7" s="19">
-        <v>14</v>
-      </c>
-      <c r="T7" s="50">
-        <f>IF(ISBLANK(U7),0,ROUND((S7-U7)*(R7/S7),0))</f>
+      <c r="S7" s="68">
+        <v>17</v>
+      </c>
+      <c r="T7" s="19">
+        <v>18</v>
+      </c>
+      <c r="U7" s="50">
+        <f>IF(ISBLANK(V7),0,ROUND((T7-V7)*(S7/T7),0))</f>
         <v>0</v>
       </c>
-      <c r="U7" s="23"/>
-      <c r="V7" s="49"/>
-      <c r="Y7" s="15">
-        <f>T7/ROUND(R7,0)</f>
+      <c r="V7" s="23"/>
+      <c r="W7" s="49"/>
+      <c r="Z7" s="15">
+        <f>U7/ROUND(S7,0)</f>
         <v>0</v>
       </c>
-      <c r="Z7" s="15">
-        <f>Y7*J7</f>
+      <c r="AA7" s="15">
+        <f>Z7*L7</f>
         <v>0</v>
       </c>
-      <c r="AB7" s="1" t="s">
+      <c r="AC7" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:28" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:29" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="B8" s="9"/>
       <c r="C8" s="10"/>
@@ -1355,53 +1372,55 @@
       <c r="G8" s="11"/>
       <c r="H8" s="11"/>
       <c r="I8" s="11"/>
-      <c r="J8" s="29"/>
-      <c r="K8" s="29"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="25"/>
-      <c r="N8" s="11"/>
-      <c r="O8" s="14"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="29"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="25"/>
+      <c r="O8" s="11"/>
       <c r="P8" s="14"/>
       <c r="Q8" s="14"/>
-      <c r="R8" s="69"/>
-      <c r="S8" s="20"/>
+      <c r="R8" s="14"/>
+      <c r="S8" s="69"/>
       <c r="T8" s="20"/>
-      <c r="U8" s="21" t="str">
-        <f>CONCATENATE(C8," ",G8, " ",L8)</f>
+      <c r="U8" s="20"/>
+      <c r="V8" s="21" t="str">
+        <f>CONCATENATE(C8," ",G8, " ",M8)</f>
         <v xml:space="preserve">  </v>
       </c>
-      <c r="V8" s="22">
-        <f t="shared" ref="V8" si="0">H8</f>
+      <c r="W8" s="22">
+        <f t="shared" ref="W8" si="0">H8</f>
         <v>0</v>
       </c>
-      <c r="AB8" s="1" t="s">
+      <c r="AC8" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="U9" s="6"/>
-      <c r="AB9" s="1" t="s">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="V9" s="6"/>
+      <c r="AC9" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="U10" s="6"/>
-    </row>
-    <row r="12" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="V10" s="6"/>
+    </row>
+    <row r="12" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
-      <c r="J12" s="30"/>
-      <c r="K12" s="30"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="26"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="30"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="T5:V5"/>
-    <mergeCell ref="B5:R5"/>
-    <mergeCell ref="B1:V1"/>
-    <mergeCell ref="B2:V2"/>
+    <mergeCell ref="U5:W5"/>
+    <mergeCell ref="B5:S5"/>
+    <mergeCell ref="B1:W1"/>
+    <mergeCell ref="B2:W2"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1450,53 +1469,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="78" t="str">
-        <f>'STAFF LIST'!B1:V1</f>
+      <c r="B1" s="79" t="str">
+        <f>'STAFF LIST'!B1:W1</f>
         <v>713H CLAIMS FOR VENDOR NAME</v>
       </c>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="78"/>
-      <c r="I1" s="78"/>
-      <c r="J1" s="78"/>
-      <c r="K1" s="78"/>
-      <c r="L1" s="78"/>
-      <c r="M1" s="78"/>
-      <c r="N1" s="78"/>
-      <c r="O1" s="78"/>
-      <c r="P1" s="78"/>
-      <c r="Q1" s="78"/>
-      <c r="R1" s="78"/>
-      <c r="S1" s="78"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="79"/>
+      <c r="J1" s="79"/>
+      <c r="K1" s="79"/>
+      <c r="L1" s="79"/>
+      <c r="M1" s="79"/>
+      <c r="N1" s="79"/>
+      <c r="O1" s="79"/>
+      <c r="P1" s="79"/>
+      <c r="Q1" s="79"/>
+      <c r="R1" s="79"/>
+      <c r="S1" s="79"/>
       <c r="Y1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="79" t="str">
-        <f>'STAFF LIST'!B2:V2</f>
+      <c r="B2" s="80" t="str">
+        <f>'STAFF LIST'!B2:W2</f>
         <v>Aug-16 to Sep-16</v>
       </c>
-      <c r="C2" s="79"/>
-      <c r="D2" s="79"/>
-      <c r="E2" s="79"/>
-      <c r="F2" s="79"/>
-      <c r="G2" s="79"/>
-      <c r="H2" s="79"/>
-      <c r="I2" s="79"/>
-      <c r="J2" s="79"/>
-      <c r="K2" s="79"/>
-      <c r="L2" s="79"/>
-      <c r="M2" s="79"/>
-      <c r="N2" s="79"/>
-      <c r="O2" s="79"/>
-      <c r="P2" s="79"/>
-      <c r="Q2" s="79"/>
-      <c r="R2" s="79"/>
-      <c r="S2" s="79"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
+      <c r="J2" s="80"/>
+      <c r="K2" s="80"/>
+      <c r="L2" s="80"/>
+      <c r="M2" s="80"/>
+      <c r="N2" s="80"/>
+      <c r="O2" s="80"/>
+      <c r="P2" s="80"/>
+      <c r="Q2" s="80"/>
+      <c r="R2" s="80"/>
+      <c r="S2" s="80"/>
       <c r="Y2" s="1" t="s">
         <v>15</v>
       </c>
@@ -1545,28 +1564,28 @@
       </c>
     </row>
     <row r="5" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="80" t="s">
+      <c r="B5" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="81"/>
-      <c r="D5" s="81"/>
-      <c r="E5" s="81"/>
-      <c r="F5" s="81"/>
-      <c r="G5" s="81"/>
-      <c r="H5" s="81"/>
-      <c r="I5" s="81"/>
-      <c r="J5" s="81"/>
-      <c r="K5" s="81"/>
-      <c r="L5" s="81"/>
-      <c r="M5" s="81"/>
-      <c r="N5" s="81"/>
-      <c r="O5" s="81"/>
-      <c r="P5" s="81"/>
-      <c r="Q5" s="82" t="s">
+      <c r="C5" s="82"/>
+      <c r="D5" s="82"/>
+      <c r="E5" s="82"/>
+      <c r="F5" s="82"/>
+      <c r="G5" s="82"/>
+      <c r="H5" s="82"/>
+      <c r="I5" s="82"/>
+      <c r="J5" s="82"/>
+      <c r="K5" s="82"/>
+      <c r="L5" s="82"/>
+      <c r="M5" s="82"/>
+      <c r="N5" s="82"/>
+      <c r="O5" s="82"/>
+      <c r="P5" s="82"/>
+      <c r="Q5" s="83" t="s">
         <v>10</v>
       </c>
-      <c r="R5" s="82"/>
-      <c r="S5" s="83"/>
+      <c r="R5" s="83"/>
+      <c r="S5" s="84"/>
       <c r="Y5" s="1" t="s">
         <v>15</v>
       </c>

</xml_diff>